<commit_message>
pós-processamento dos classificadores efetuado
</commit_message>
<xml_diff>
--- a/Python/54BND_knn.xlsx
+++ b/Python/54BND_knn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F3AA0-EB39-47DC-8C17-42987D6D17DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA5221-3693-475D-8B40-362E870EC4F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,11 +109,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -121,6 +118,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,6 +140,1096 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'54BND'!$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'54BND'!$I$28:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'54BND'!$I$29:$N$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.7407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7592592592592593</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7592592592592593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7592592592592593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72222222222222221</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0B4-4DF6-871E-E14F318B58E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'54BND'!$H$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'54BND'!$I$28:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'54BND'!$I$30:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.72222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70370370370370372</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70370370370370372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70370370370370372</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68518518518518523</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B0B4-4DF6-871E-E14F318B58E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'54BND'!$H$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'54BND'!$I$28:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'54BND'!$I$31:$N$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.48148148148148151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53703703703703709</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59259259259259256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B0B4-4DF6-871E-E14F318B58E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2071713792"/>
+        <c:axId val="2007636032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2071713792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2007636032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2007636032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2071713792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4E34BF2-04A5-498B-841A-FC180379DF83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,96 +1553,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H28" sqref="H28:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>15</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>14</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>13</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>12</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>11</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>10</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>15</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>14</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>13</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>12</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>10</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="2">
         <v>15</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="2">
         <v>14</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="2">
         <v>13</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q1" s="2">
         <v>12</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R1" s="2">
         <v>11</v>
       </c>
-      <c r="S1" s="3">
+      <c r="S1" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1376,7 +2470,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1435,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1494,7 +2588,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1553,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1612,7 +2706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1671,7 +2765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1730,7 +2824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1789,7 +2883,7 @@
         <v>0.59259259259259256</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +2942,7 @@
         <v>0.6071428571428571</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1905,6 +2999,107 @@
       </c>
       <c r="S25">
         <v>0.57692307692307687</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>2</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3</v>
+      </c>
+      <c r="L28" s="5">
+        <v>4</v>
+      </c>
+      <c r="M28" s="5">
+        <v>5</v>
+      </c>
+      <c r="N28" s="5">
+        <v>6</v>
+      </c>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H29" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="I29">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="J29">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="K29">
+        <v>0.7592592592592593</v>
+      </c>
+      <c r="L29">
+        <v>0.7592592592592593</v>
+      </c>
+      <c r="M29">
+        <v>0.7592592592592593</v>
+      </c>
+      <c r="N29">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H30" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="I30">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="J30">
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="K30">
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="L30">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="M30">
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="N30">
+        <v>0.68518518518518523</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H31" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I31">
+        <v>0.48148148148148151</v>
+      </c>
+      <c r="J31">
+        <v>0.53703703703703709</v>
+      </c>
+      <c r="K31">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="L31">
+        <v>0.57407407407407407</v>
+      </c>
+      <c r="M31">
+        <v>0.57407407407407407</v>
+      </c>
+      <c r="N31">
+        <v>0.59259259259259256</v>
       </c>
     </row>
   </sheetData>
@@ -1914,5 +3109,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>